<commit_message>
pdf functionality is working perfectly
</commit_message>
<xml_diff>
--- a/orders_dh.xlsx
+++ b/orders_dh.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2725,6 +2725,1001 @@
         <v>740.12</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O13" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P13" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R13" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T13" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U13" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V13" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R14" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T14" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U14" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V14" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O15" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P15" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R15" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T15" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U15" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V15" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P16" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R16" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T16" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U16" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V16" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O17" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P17" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R17" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T17" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U17" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V17" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
made various test files for shipping
</commit_message>
<xml_diff>
--- a/orders_dh.xlsx
+++ b/orders_dh.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,6 +548,46 @@
       <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Total Price (USD)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Carrier</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Service</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Shipping Rate (USD)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Tracking Code</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Tracking URL</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Label URL</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Parcel Size</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Parcel Key</t>
         </is>
       </c>
     </row>
@@ -3720,6 +3760,414 @@
         <v>740.12</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O18" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R18" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T18" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U18" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V18" t="n">
+        <v>740.12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>33fae5b6</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-08-05 04:05:02</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>darkwangduck</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Ben Eckart</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3873 Patterson Ave</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Oakland</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>94619-2029</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>wax melts -  Punishers</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>[Bulk option] 300g - Wax Skulls</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>UPS 2 Day</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>A0FAB2C4179732922AEEE4924B0E9743AC2EEF18</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP PUBLIC KEY BLOCK-----
+mQINBFnEIiEBEADMrm4vb5QBopQe5Jq7fM/B0qoiICt0+H1NzbiY7vyG8a4LmOMB
+IIdfSjlfhdRC3snzL1t+cYZR13/msqlIRCjHlamGgHCoOaJftd0f+lUdopVWKF+c
+RGMaEfnN4ZsS2VFTZnlGvIP6roZtNazD7XoGprGWqht30WUw0gkzgn3540zYJmMO
+ijz/i9BFYhvAtMo9ABzdxMkK6kdNr4d7QiuhETw4n8NhgPro7BvciQxVDwvDKUAE
+49NUPpXTgnEugemQS4E3hXZ6O5YbBVsSZJCKOd20tkZBAYUKYd834TEcJ7V8I7L/
+xOeAiwQYHCZiIYpdO6BKpPl2XKHUyCcHp47jgN+jJpsYSyJrlN3llt1mc1bl42ei
+smql9y4PiLXo4uhQoaJrDNc/MeD7XMFYrQXpuckVNXeu/EhwngQZrDuznPv4ncOz
+qfc6Lw73vAioUli3Rpfv3LVFmtJbXHJHcSo6/5+bLLznT113XrgBoZaAaVtAVaiV
+1kDX5PE0b0mzOw7mRNzw9Q+gVmSiPbO//JOpJfqIaZuJ51umjOyNlgQ1VQ+1TVY7
+s75IPnnZb6/J3AzZjh3qB4JrK3E0WydgeM9vrqKzOv5G+Ro1Wwb4QF4O1GrF9e7u
+Fa+hzyMO9ASRINISR3+5RCvmghxrYyBRfDoQPwlYRryA4tkZ2BtU+AeEMQARAQAB
+tCBCYXJiYXJhIDxiNHJiNHI0QHByb3Rvbm1haWwuY29tPokCOAQTAQIAIgUCWcQi
+IQIbAwYLCQgHAwIGFQgCCQoLBBYCAwECHgECF4AACgkQSw6XQ6wu7xhIehAAtxfI
+/WFCwZzyyailymwphJm8EYW0RU157r5mm/NB5E4W4SUlibnLFk+ThImAfhn2kmW8
+2a0O39jzgWfqWhwCxsbSrDsg3eC9X5jdkZIid9e1C5oZVGVDeA3ScowxApFAdEZp
+nskR05uw72zK8TgCLlunNwAx+BBk9pzl3eys2Xgwj/+fQhOzFhIVvKUKSpA9MZ5c
+WaE8w+BD0SPHNof+btwoSzy1FeHhAZ2umaesXIsAJI+jGxPQi7h/82k9ZJ5jitfw
+gfSKIYEptIS2RO4L0hDVYb0Spy1q5pfYDYobh7QaEVxQ1emijixZuPwhRJZUOaQj
++6sC1yWDifKE4Td135tn5MBQkjFXziTWQRVP8aJpZYeAq4XO3g4miBc/X3f+HTrz
+3c1NCJ05SjJ/7kufzup2rmxHhXF9qIRKtr84u/PJrV0KftSdxbuV6S+l7M2c9BnP
+mjrJse4g/7pRowzQSljzXAlSy8B9sIONM07HhRJloqbw022u+nlpFLoR9gzkgrDp
+1zVm7wzjk7X78p/mWLqf9iqqovtHbx61Uja4Rc6I3GxKBNGruifVv0R5CL1pQe6J
+VnUZ3OpWKa4xHX0/EOywacvCFgfl4UlZWX8fBbZZWvsVKhzXpCSD2WqKjAYQrRi+
+KwG8AgA+WOKLJOzwUshK4a0OvLiGVugPK6Vj0165Ag0EWcQiIQEQAMoPxzzljR7Y
+xW1/aQ5udRQ1CkibW8FAOR4GuyTJmR2lLXU5Z4k+a6E4gIyM2bZs27LKG1Xc8dny
+e7VuaIMkntgTnHIn8qqiU2s2nTEXDGg4D9zDLpsQWv+ABs5oByEK46IAnI62IUSY
+Lb2pFTMvEZ+FR2Zk3foILg4znoyXAlzsHIhmyuvm6j2qbOV0zW7QnUg1ZmngPrhM
+URgFU/+qN6/DJKcFXMAAEjxTaby2HWGxWPt5+vfTJAMbQVZIjdvSlQ+tEf0XWT7g
+3qxx+DU5/x4uVh4wW9tOiiK/okE0rEoaIWwltu0A8c2u80kfiSv9zGOQ4xNLfPQr
+YrlNKNPKIa2qgiHHIf7rt+Myxn9E6tFUJ5ZtB95i28DydYQTZjcDaax49zo9j2q+
+Emj7NTZ8ea9CEGL358jLUOcCpwiz57pSlTUvowu8ckFfTNm7xLjSddbN24KMdPvY
+lJHMc8CwKi9R0PSJJzrPdj5enFVPazGgMfH8xnR6FWCvPVhQDJRZQViC8+y1NCVo
++Vc/FWwDp5JsagH63lNj+d8J6VvgZ6dKTfR3TBj27586N2WuD0oox8etO7BqRmX0
+f/39nOUm2wFnhSRi6DcucDeO+QReq+7T7W+zXQc/mUb8xFgUKIVAEfRQCsjXbLNk
+/eS5MdEWAuMMuomAvNkPSu+IYRhMjVZdABEBAAGJAh8EGAECAAkFAlnEIiECGwwA
+CgkQSw6XQ6wu7xgoZhAAu9qsEM1czZDD6qqwGRv7zMAnTireGvRmE60Y1NwSVowq
+Wv2YNDzQLr1FcCcdZAuLm85OOl5TMaeAncjpdvWiSKlFtEyn4qAvWWxLPOB+Iue6
+3y65h7+/ZzWjRUEPamTJjZf/87DY5TZiSWSzMMvAyugGGpPwnsu0KfWjinUX2Nfm
+EVcj9NWkpNkna+sS7pq7tDN1q+8Lm3dIOv9CEnxxI9jgi1RUiGELthq46lHadWux
+x0UV1yvn8QtAajRAuqZYgwi7oLYsa0n0nEgjEq5H2Mn5j1m5LwlFbrRcZb2v+5FB
+fgcxs2VW3nbEOUDtlxCD3ySE2jHksxjRoJTuQRPPXDLAphoqV3OrJnaSl6UzWgaB
+BjX++NXdb5TVAzDNRDQicSbP7SWdtTQD/G5dR8Py19DQF97Yiolw+WYbwSBde3H5
+e2ecnJGObVWehfZ0H4hb7ekgWH3Gw8RFExd6ydSt0Beaf/B8ZPvw1LZ8ZN2qaeFt
+EOgFxUn59D1uzxxXJNw9zop1mUfELfcrKD4vgxIZXrLWw1n9i8z6Au1eud+znOZM
+rBb0Fx0i0pTVF/QZ98UQ0w4+cyGLS9VtYZ0QZFY3e4SbLfEMNoidPc/JTNrVXzxF
+gW5Qju7JUghRY7ti5QcNXZDu1WFzwYaTUrD4ZBVKf4azSWOt99i0EzBmDSvKdiM=
+=qzG7
+-----END PGP PUBLIC KEY BLOCK-----</t>
+        </is>
+      </c>
+      <c r="O19" s="3" t="inlineStr">
+        <is>
+          <t>'-----BEGIN PGP MESSAGE-----
+hQIMA1XtIn7QB2h8ARAAoRfX/zZ5DShXY7dBkk428DjLovHsBgTvzuKkQerrBI1y
+NJQSXMdX+71vJFaesjojHamv7kcBlBDYkZc7CETOsekDCJPC7a1OBGFZ20AV39Ep
+uni7vbLrR0TJ/d0o+t66bTf7NJ2ZeRlertIgiJjUtVwobgOZls/uwpVOEWRZ3g76
++9M5aJtzCxnQN2gKdVqVvgnNNGCDE1aZw9TO1AXyK/Z51vWYrIPbQ2fcWHhE44Ya
+6YslLxTHEqqN0OIBR5U/VxZ52OegmOcOL9YzUp9Coh+fNyczRvCrM1pjGbODffkX
+j4JaNPaUxbtbnZfGg0B6U27U1GN3PC793F5c7RoicM5RssIUC4tBP+/YatTnIRkv
+x//2BZ7MXdIn0OVUkdDKZEadJMzXIpnMTlVfFKDbBY/j+ghf7wBFTjzVk6teJEj2
+Azh54zkLLwldWHxAX/uSotNQ4/zUqdi3PRIqECp4wifx2bNLqXE3Depu2LVtdfcV
+CLLxuyPv0T7MNqdsRURqqvHDglbU0WTJMFPDhz5DAFNpNNor6PjUxPaP0bOvRxiN
+jIh4qGjiB6sm+38bYBa8SVH4BaqXUnmwoWTGzrAuatxfYqIAdx0BRzFqM5wbS4Ed
+KEE9Uonr61I/ZntghQ0f1zqO5kCEraY993z6O3ScEZIXPVaOXfY3TojHW7ApNlqF
+AgwDVjkqg7iqkkQBEACDd5+NgO6bnOgzEq0nKHXxnNv5zwG6f8Ts0BnXY34RZANn
+3UmRYziOV8naxlKZbHulix33NC+m/3ofaDDL/9UQzPSvUUwWWmkb5/3U70c66KCN
+jXWLUyXgGAi1EObCgzA+8Nd2QwpVgJ5QXY/aTHTwJjoiL82z0gIuqZ/loVzlbyB+
+S6L0QU7Tec1pDnAGu4VMKmaQ7l17xAN7AkxVRK/cxbMf9KIyf5m3W8d97LBuCtdW
+yfqpKYDD/jBXQ/Ta1xQzj5kfKLpKVqTnaFC3gsMUzI9e9NCdsswwKJ38qAjAyTV+
+xPTxJberF+P6q2ufsCshgrCoNig1Uu0ZMI4bcr6TLouzg05UIzf+Z7x23YQihknx
+n3BVRyW7DWpgmuxavLdoyQgIqlnhWTm7LOel0XBMP8q8LKyoOaxYyb3QGlEuDcNE
+HDtkqNtPDmBJwRg2UkCy/VsagqCUb+pl/mi81W/+g6fhMkdZGladTuI2U6e1fABC
+BG0l2v68n+1GXBit7nwFP5uZhjjw4tptk7MQflSQFGsGWkh4yjEJqtd/tsF+hSJE
++A/AD00EJy5a/UGl0ZAdq71e1TQZr3NJQGFILTUvraVX8eVJzEBKmW0bHexJ9Doi
+tMIihd896jx/lwbb5IFUNRUeVdST/VrxCz2DwnjF0HXqiAU98FWbTzkTD1vf0tLp
+AQpXPDCcwmx0uhsBRFC8hcmgzKtjDA+fmxKVO96yzTbDgrzxyaotGL+QTOoNaEcC
+h3/SmaEPdg5/0++gzrIzH2dvD8ScurTQ4o47ygL0swUHkIX4CY+Xwo4Hnh9MIJwi
+AyEFIO1gLlq1yLMCw2qAmCfBU3lfZ+EONZdiMu5gHf/CTmUmV/zY2Ar7V7J7Orb3
+AVzX3Sexx3AL4wscU9CDjywsEWQB9CEfHA88K9N5/ALTms1kecR0KP2XXvltiBLA
+haQP0m8bv0SesVii/Kfb9v2HyChBa3NN18c6Ks3tN/aFnH4v5wuYIGDtvICTCG+0
+A+UNZyAkbg/Ykr4X5wPI33aWGPL6viBpO+3i+5mir1PLBPnRcdmazIF54bSs2gur
+lNce+RctppqOhpul529vlc42K1FEuzaTm4W9D1Z96m4PsMezjhMr1gMUEa598628
+t9V699r540f5Qv93NBNe7UFgWJceaIWJzhvM55zKtXBLw7LU8+oxWQ64mpVRgoZv
+BdjiRO6RoFCnTUGmCzuV9pKddZ7H7dD+VDovk6QI7mVG755+9Iw49B2o3doD6Ft2
+NJFE3Jrgl4ZHZMY+boc3x97j4tK+bGBqJ5k2rJFtbBEMJO/ymB4EhgYD8VnXFftZ
+j25V52NyBuCp75CsMhn3fhCtrioln9X4ivbk+FqQxpiVAxOyepjD5IJUQDW3xErw
+SQAqQoUr+H9BMtWjEHfp00pmO/Uzq/TD+ohP0nsvL3Vh8gPYeYQXjbRfeg76a9v+
+hLREyIPXsQSeFZ82XtVzkklv5UZqMmxJDrGI5o7Eduql1iO34qlgpfFyHSLrembi
+B9xnITM9xHNJ7CrAXzLEjKLrynKPT0etW/GWBeKk4uSKX8MEZ4I=
+=mO3k
+-----END PGP MESSAGE-----
+-----BEGIN PGP MESSAGE-----
+hQIMA1Y5KoO4qpJEAQ//R26qF9UY/Sh0e0HyCsD+kvhUWxNWOdoD3YJSLZfb1bu1
+u3J/v0nQUoplzMC/N1oxTf0ZBgQFUSRXT0GTzmQNZknwsZDPZMIPs9n9JTrAo5yq
+GDF2CrUrQKJJz8pMZ0r2eaig7lUmrdN4/Ruve66rrF2vxwDa4j2kR+HTq3pfNoof
+UwAS8ZhXneRYLCP+BNV41ea5eWHeqj8cVGJnW0KIm34qfCLJKrs4J3C8KjQQsAHA
+SmYDLhu/gntZPN1v/+zxZ0fXltkzeN99HeXJmnyLRd36YmgST34Y+OfrACpx2PSn
+aNBhCVFLvt3wN+AeSFOAZUIMAvwdNtvSOgeGq3FCgeHpE2R9I3626SssufVfDgpq
+bwxHiG37wLF7GSlIo0wOcuqlmuKBa7b2q9gINefA2+FSpU6CrvNwNLCiO6yBDmAg
+Ldv9bXKEw6ZbNhTGICQ3FMwkB9mDDdJ+qzCS2oVsC91nvvnB8huVEqNlA06URBEX
+564x/cdBRiqCHaRNXii7eNNsrupTJJCEiY3cq8rewTH5Stc8Y/Ju2E8a7uHUJszR
+GtxgSpvJlvXRm41eX/SJ1Jel2gIUdKmNX2Lq9ZU0Ff8HUPCZ5QJHR4rpf5yY6IJk
+7SSqLMI7s8/UhUm9rSwLEhChJBZt8Gbg2UH9Swx/IIvEmNbcq44rIrjgSY9t0OPS
+bwFoThLJ8SFWLEZ1owP2ws3kzWZOkRiSRtIBY/HBeTXziHpOsVp1Gd122DMGoUom
+/FFe8hL2r9iJXdn9FxoJ3z/vsBnVbEZqNdz6ORG9rQDSEKVVbmT+0GM4IThQklYs
+cTS7RKCq++tUWmJvn9chfQ==
+=OUrC
+-----END PGP MESSAGE-----</t>
+        </is>
+      </c>
+      <c r="P19" s="3" t="inlineStr">
+        <is>
+          <t>'Order processed by vendor.
+Order accepted by vendor.</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>2.334189202708</v>
+      </c>
+      <c r="R19" t="n">
+        <v>700.12</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.133382240155</v>
+      </c>
+      <c r="T19" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="U19" t="n">
+        <v>2.467571442863</v>
+      </c>
+      <c r="V19" t="n">
+        <v>740.12</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>SMALLEST</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>PARCEL_3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>